<commit_message>
modify titles and data in Negociado de la Policia
</commit_message>
<xml_diff>
--- a/data/Negociado_de_Policia/npprDS_tiposdelitos.xlsx
+++ b/data/Negociado_de_Policia/npprDS_tiposdelitos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orlan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnper\Documents\ViolenciaGeneroPR\data\Negociado_de_Policia\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6260E7E4-683C-497F-A522-8AF317072503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
@@ -19,17 +20,28 @@
     <sheet name="2023" sheetId="5" r:id="rId5"/>
     <sheet name="2024" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
   <si>
     <t>Delitos</t>
   </si>
@@ -46,9 +58,6 @@
     <t>Sodomia</t>
   </si>
   <si>
-    <t>Actos Lasivos</t>
-  </si>
-  <si>
     <t>Incesto</t>
   </si>
   <si>
@@ -77,12 +86,15 @@
   </si>
   <si>
     <t>Hostigamiento Sexual</t>
+  </si>
+  <si>
+    <t>Actos Lascivos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,17 +405,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -425,7 +439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -436,9 +450,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>491</v>
@@ -447,9 +461,9 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>13</v>
@@ -458,9 +472,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>70</v>
@@ -469,14 +483,91 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
         <v>0</v>
       </c>
     </row>
@@ -486,17 +577,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="A14:C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,7 +600,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -518,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -529,9 +622,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>296</v>
@@ -540,9 +633,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -551,9 +644,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>58</v>
@@ -562,15 +655,92 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -579,17 +749,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="A14:C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -611,7 +783,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -622,9 +794,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>514</v>
@@ -633,9 +805,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -644,9 +816,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>66</v>
@@ -655,14 +827,91 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
         <v>0</v>
       </c>
     </row>
@@ -672,17 +921,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="A14:C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -704,7 +955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -715,9 +966,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>590</v>
@@ -726,9 +977,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -737,9 +988,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>58</v>
@@ -748,9 +999,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -759,9 +1010,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>19</v>
@@ -770,9 +1021,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>13</v>
@@ -781,9 +1032,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -792,14 +1043,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
         <v>0</v>
       </c>
     </row>
@@ -809,17 +1093,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="A14:C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -830,7 +1116,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -841,7 +1127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -852,9 +1138,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>551</v>
@@ -863,9 +1149,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>25</v>
@@ -874,9 +1160,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>36</v>
@@ -885,9 +1171,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -896,9 +1182,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>29</v>
@@ -907,9 +1193,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>39</v>
@@ -918,9 +1204,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>13</v>
@@ -929,26 +1215,48 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -957,17 +1265,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -978,7 +1288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -989,7 +1299,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1000,9 +1310,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>503</v>
@@ -1011,9 +1321,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1022,9 +1332,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>20</v>
@@ -1033,9 +1343,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1044,9 +1354,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>17</v>
@@ -1055,9 +1365,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>88</v>
@@ -1066,9 +1376,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -1077,25 +1387,47 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
+      <c r="C14">
         <v>2</v>
       </c>
     </row>

</xml_diff>